<commit_message>
docs: Atualização de conteúdo bl10.1
</commit_message>
<xml_diff>
--- a/SoftSkills/Inteligência Emocional - História da Vida.xlsx
+++ b/SoftSkills/Inteligência Emocional - História da Vida.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t xml:space="preserve">História da Vida</t>
   </si>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">Momentos positivos</t>
   </si>
   <si>
-    <t xml:space="preserve">Natal em família
+    <t xml:space="preserve">Passeios, viagens, e Natal em família.
 </t>
   </si>
   <si>
@@ -72,10 +72,10 @@
     <t xml:space="preserve">Meu primeiro trabalho com carteira assinada. Cursei contabilidade e comecei a trabalhar na área. </t>
   </si>
   <si>
-    <t xml:space="preserve">Contratado para trabalhar no RH de uma multinacional, morei dois anos em outra cidade, me formei em administração, nascimento do meu filho e casei. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decidir fazer transição de carreira e começar a estudar na Trybe.</t>
+    <t xml:space="preserve">Contratado para trabalhar no RH de uma multinacional, morei dois anos em outra cidade, me formei em administração, nascimento do meu filho e casei com a meu amor platônico da época de escola. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decidi fazer transição de carreira e começar a estudar na Trybe.</t>
   </si>
   <si>
     <t xml:space="preserve">Momentos negativos</t>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t xml:space="preserve">Repeti de série dois anos e não consegui entrar para a marinha.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comprei um carro parcelado que bateu o motor e fiquei mais com ele parado, e pagando as parcelas, do que com ele andando. </t>
   </si>
   <si>
     <t xml:space="preserve">Sair da empresa que atuava em RH, trabalhei com administração em uma empresa que minava muito a energia, momentos econômicos mais difíceis e pandemia.  </t>
@@ -409,10 +412,10 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.06"/>
@@ -467,7 +470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -507,12 +510,14 @@
       <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="F4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -521,23 +526,23 @@
     </row>
     <row r="5" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -569,7 +574,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="26.59"/>
@@ -577,7 +582,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -692,7 +697,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="6"/>
@@ -759,7 +764,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="6"/>

</xml_diff>